<commit_message>
new xgb run needed
</commit_message>
<xml_diff>
--- a/Output/Classifier Inference/XGBoost/All_Data Prediction Statistics.xlsx
+++ b/Output/Classifier Inference/XGBoost/All_Data Prediction Statistics.xlsx
@@ -447,10 +447,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.001146352291107178</v>
+        <v>0.0009961605072021484</v>
       </c>
       <c r="B2" t="n">
-        <v>7.698806521874934e-07</v>
+        <v>6.69013100874512e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>